<commit_message>
A whole bunch of stuff that I should have been commiting as I went along!!!
</commit_message>
<xml_diff>
--- a/density_data/SUMP_densitydata_2018.xlsx
+++ b/density_data/SUMP_densitydata_2018.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamjohnson/Desktop/Laura/Mussels/Research/field_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamjohnson/Desktop/Laura/Hallett_Lab/Repositories/thesis-mussels/density_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94973112-90AE-484D-8007-8CDFC8FAA34A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0F3358-87FA-BD46-A951-9DDB868A2A71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2740" windowWidth="23740" windowHeight="15720" xr2:uid="{FB701106-E7F8-1F4F-B71A-32F5598F8F5A}"/>
+    <workbookView xWindow="2380" yWindow="800" windowWidth="26960" windowHeight="15720" xr2:uid="{FB701106-E7F8-1F4F-B71A-32F5598F8F5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Density_Data" sheetId="1" r:id="rId1"/>
     <sheet name="Metadata" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="80">
   <si>
     <t>obs_id</t>
   </si>
@@ -148,9 +148,6 @@
     <t>BKY0302</t>
   </si>
   <si>
-    <t>Lots of Asian clams around. Large M. falcata tucked into bedrock shelf on stream right. Lots of deposition of fines; mussels only visible due to exposed apertures.</t>
-  </si>
-  <si>
     <t>BKY0401</t>
   </si>
   <si>
@@ -217,15 +214,6 @@
     <t>TIL0302</t>
   </si>
   <si>
-    <t>Primarily boulder (40%) and bedrock (40%) with equal cobble and sand (10% each) that has settled into notches</t>
-  </si>
-  <si>
-    <t>TIL0303</t>
-  </si>
-  <si>
-    <t>Primarily bedrock (80%) with material settled into an eroded notch (15% sand, 5% gravel)</t>
-  </si>
-  <si>
     <t>COW0101</t>
   </si>
   <si>
@@ -256,9 +244,6 @@
     <t>Western pearlshell. Found on stream left on the side of a boulder in the fast water section we ended in.</t>
   </si>
   <si>
-    <t>COW0202</t>
-  </si>
-  <si>
     <t>In m^2. For visual observations, area was recorded as the minimum amount of stream area that held the observed mussels within an aggregation. 0.25 m^2 is the smallest possible value recorded, although in reality the streambed occupied by solitary mussels is less than this minimum value. For observations that were systematically sampled, area refers to the size of the mussel bed as determined by animals available at the substrate surface.</t>
   </si>
   <si>
@@ -266,6 +251,27 @@
   </si>
   <si>
     <t xml:space="preserve">Data recorded during the summer of 2018 in the South Umpqua River and Cow Creek as part of Laura Johnson's masters thesis research. All data represents records of live animals (not shell data). </t>
+  </si>
+  <si>
+    <t>BKY0303</t>
+  </si>
+  <si>
+    <t>BKY0304</t>
+  </si>
+  <si>
+    <t>Lots of sand and fines; this is a deposition zone. Landowner Alvin H. Jr. Helegeson id'd this location as site of large mussel bed when he was a boy (50+ years ago). On stream right just off bedrock shelf. HUGE asian clam graveyard and 1000s of live C. fluminea.</t>
+  </si>
+  <si>
+    <t>On stream left just upstream from riffle; about 100 m upstream from large cobble bar. Sparse to no streamside vegetation. Widely spaced animals interspersed within large gravel and cobble- several meters b/w mussels.</t>
+  </si>
+  <si>
+    <t>Lots of Asian clams around. Large M. falcata tucked into bedrock shelf on stream right. Lots of deposition of fines; mussels only visible due to exposed apertures. GPS point estimated using ArcMap 10.5.</t>
+  </si>
+  <si>
+    <t>Combined AGG01 and AGG02 for data analyses and visualization. AGGs were located 6 m apart in bedrock notches with deposition. Agg 01 contained 50 mussels in 2 m^2 area and was primarily boulder (40%) and bedrock (40%) with equal cobble and sand (10% each), whereas Agg 02 contained 10 mussels in a 0.5 m^2 area and was primarily bedrock (80%) with material settled into the eroded notch (15% sand, 5% gravel)</t>
+  </si>
+  <si>
+    <t>COW0201</t>
   </si>
 </sst>
 </file>
@@ -281,18 +287,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -307,13 +307,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -629,15 +628,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D21F69-9E09-8F42-8303-9DE021CDA323}">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
@@ -722,10 +724,10 @@
         <v>0.29629630000000001</v>
       </c>
       <c r="K2">
-        <v>42.934260000000002</v>
+        <v>43.079267999999999</v>
       </c>
       <c r="L2">
-        <v>-123.03869</v>
+        <v>-123.38822999999999</v>
       </c>
       <c r="M2" t="s">
         <v>21</v>
@@ -769,7 +771,7 @@
         <v>15</v>
       </c>
       <c r="J3">
-        <f>G3/I3</f>
+        <f t="shared" ref="J3:J22" si="0">G3/I3</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="K3">
@@ -788,7 +790,7 @@
         <v>43265</v>
       </c>
       <c r="P3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
@@ -820,7 +822,7 @@
         <v>60</v>
       </c>
       <c r="J4">
-        <f>G4/I4</f>
+        <f t="shared" si="0"/>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="K4">
@@ -871,7 +873,7 @@
         <v>7.5</v>
       </c>
       <c r="J5">
-        <f>G5/I5</f>
+        <f t="shared" si="0"/>
         <v>0.53333333333333333</v>
       </c>
       <c r="K5">
@@ -922,7 +924,7 @@
         <v>75</v>
       </c>
       <c r="J6">
-        <f>G6/I6</f>
+        <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
       <c r="K6">
@@ -973,7 +975,7 @@
         <v>30</v>
       </c>
       <c r="J7">
-        <f>G7/I7</f>
+        <f t="shared" si="0"/>
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="K7">
@@ -992,12 +994,12 @@
         <v>43303</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -1015,40 +1017,40 @@
         <v>19</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H8" t="s">
         <v>20</v>
       </c>
       <c r="I8">
-        <v>0.25</v>
-      </c>
-      <c r="J8" s="4">
-        <f>G8/I8</f>
-        <v>4</v>
+        <v>200</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
       </c>
       <c r="K8">
-        <v>43.048726000000002</v>
+        <v>43.062443999999999</v>
       </c>
       <c r="L8">
-        <v>-123.328327</v>
+        <v>-123.354012</v>
       </c>
       <c r="M8" t="s">
         <v>21</v>
       </c>
       <c r="N8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="O8" s="1">
-        <v>43355</v>
-      </c>
-      <c r="P8" t="s">
-        <v>40</v>
+        <v>43302</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
@@ -1066,40 +1068,40 @@
         <v>19</v>
       </c>
       <c r="G9">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H9" t="s">
         <v>20</v>
       </c>
       <c r="I9">
-        <v>10</v>
+        <v>210</v>
       </c>
       <c r="J9">
-        <f>G9/I9</f>
-        <v>0.2</v>
+        <f t="shared" si="0"/>
+        <v>5.7142857142857141E-2</v>
       </c>
       <c r="K9">
-        <v>43.047362</v>
+        <v>43.063693999999998</v>
       </c>
       <c r="L9">
-        <v>-123.32917999999999</v>
+        <v>-123.352068</v>
       </c>
       <c r="M9" t="s">
         <v>21</v>
       </c>
       <c r="N9" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="O9" s="1">
-        <v>43355</v>
-      </c>
-      <c r="P9" t="s">
-        <v>42</v>
+        <v>43302</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
@@ -1125,12 +1127,19 @@
       <c r="I10">
         <v>0.25</v>
       </c>
-      <c r="J10" s="4">
-        <f>G10/I10</f>
+      <c r="J10" s="3">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
+      <c r="K10">
+        <v>43.048726000000002</v>
+      </c>
+      <c r="L10">
+        <v>-123.328327</v>
+      </c>
+      <c r="M10" t="s">
+        <v>21</v>
+      </c>
       <c r="N10" t="s">
         <v>33</v>
       </c>
@@ -1138,12 +1147,12 @@
         <v>43355</v>
       </c>
       <c r="P10" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -1167,17 +1176,17 @@
         <v>20</v>
       </c>
       <c r="I11">
-        <v>0.25</v>
-      </c>
-      <c r="J11" s="4">
-        <f>G11/I11</f>
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
       </c>
       <c r="K11">
-        <v>43.045456999999999</v>
+        <v>43.047269999999997</v>
       </c>
       <c r="L11">
-        <v>-123.329596</v>
+        <v>-123.328733</v>
       </c>
       <c r="M11" t="s">
         <v>21</v>
@@ -1189,63 +1198,63 @@
         <v>43355</v>
       </c>
       <c r="P11" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="G12">
-        <v>364</v>
+        <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="I12">
-        <v>52.5</v>
-      </c>
-      <c r="J12" s="4">
-        <f>G12/I12</f>
-        <v>6.9333333333333336</v>
-      </c>
-      <c r="K12">
-        <v>42.934260000000002</v>
-      </c>
-      <c r="L12">
-        <v>-123.03869</v>
+        <v>0.25</v>
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="K12" s="3">
+        <v>43.046411999999997</v>
+      </c>
+      <c r="L12" s="3">
+        <v>-123.32916899999999</v>
       </c>
       <c r="M12" t="s">
         <v>21</v>
       </c>
       <c r="N12" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="O12" s="1">
-        <v>43292</v>
+        <v>43355</v>
       </c>
       <c r="P12" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
@@ -1254,7 +1263,7 @@
         <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="E13" t="s">
         <v>18</v>
@@ -1263,7 +1272,7 @@
         <v>19</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H13" t="s">
         <v>20</v>
@@ -1271,25 +1280,32 @@
       <c r="I13">
         <v>0.25</v>
       </c>
-      <c r="J13" s="4">
-        <f>G13/I13</f>
-        <v>4</v>
-      </c>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="J13" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="K13">
+        <v>43.045456999999999</v>
+      </c>
+      <c r="L13">
+        <v>-123.329596</v>
+      </c>
+      <c r="M13" t="s">
+        <v>21</v>
+      </c>
       <c r="N13" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="O13" s="1">
-        <v>43292</v>
+        <v>43355</v>
       </c>
       <c r="P13" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
         <v>30</v>
@@ -1298,32 +1314,32 @@
         <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E14" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="F14" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="G14">
-        <v>86978</v>
+        <v>364</v>
       </c>
       <c r="H14" t="s">
         <v>26</v>
       </c>
       <c r="I14">
-        <v>931.84</v>
-      </c>
-      <c r="J14" s="4">
-        <f>G14/I14</f>
-        <v>93.340058379120876</v>
+        <v>52.5</v>
+      </c>
+      <c r="J14" s="3">
+        <f t="shared" si="0"/>
+        <v>6.9333333333333336</v>
       </c>
       <c r="K14">
-        <v>42.939444000000002</v>
+        <v>42.934260000000002</v>
       </c>
       <c r="L14">
-        <v>-123.00241</v>
+        <v>-123.03869</v>
       </c>
       <c r="M14" t="s">
         <v>21</v>
@@ -1332,15 +1348,15 @@
         <v>27</v>
       </c>
       <c r="O14" s="1">
-        <v>43297</v>
+        <v>43292</v>
       </c>
       <c r="P14" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
         <v>16</v>
@@ -1349,7 +1365,7 @@
         <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
         <v>18</v>
@@ -1358,23 +1374,23 @@
         <v>19</v>
       </c>
       <c r="G15">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="H15" t="s">
         <v>20</v>
       </c>
       <c r="I15">
-        <v>2</v>
-      </c>
-      <c r="J15" s="4">
-        <f>G15/I15</f>
-        <v>25</v>
-      </c>
-      <c r="K15">
-        <v>42.939250000000001</v>
-      </c>
-      <c r="L15">
-        <v>-123.0018</v>
+        <v>0.25</v>
+      </c>
+      <c r="J15" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="K15" s="3">
+        <v>42.933487</v>
+      </c>
+      <c r="L15" s="3">
+        <v>-123.03795</v>
       </c>
       <c r="M15" t="s">
         <v>21</v>
@@ -1383,24 +1399,24 @@
         <v>27</v>
       </c>
       <c r="O15" s="1">
-        <v>43297</v>
+        <v>43292</v>
       </c>
       <c r="P15" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16" t="s">
         <v>18</v>
@@ -1409,23 +1425,23 @@
         <v>19</v>
       </c>
       <c r="G16">
-        <v>10</v>
+        <v>86978</v>
       </c>
       <c r="H16" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="I16">
-        <v>0.5</v>
-      </c>
-      <c r="J16" s="4">
-        <f>G16/I16</f>
-        <v>20</v>
+        <v>931.84</v>
+      </c>
+      <c r="J16" s="3">
+        <f t="shared" si="0"/>
+        <v>93.340058379120876</v>
       </c>
       <c r="K16">
-        <v>42.939250000000001</v>
+        <v>42.939444000000002</v>
       </c>
       <c r="L16">
-        <v>-123.0018</v>
+        <v>-123.00241</v>
       </c>
       <c r="M16" t="s">
         <v>21</v>
@@ -1434,24 +1450,24 @@
         <v>27</v>
       </c>
       <c r="O16" s="1">
-        <v>43662</v>
+        <v>43297</v>
       </c>
       <c r="P16" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="D17" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="E17" t="s">
         <v>18</v>
@@ -1460,49 +1476,49 @@
         <v>19</v>
       </c>
       <c r="G17">
-        <v>112</v>
+        <v>60</v>
       </c>
       <c r="H17" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="I17">
-        <v>43</v>
-      </c>
-      <c r="J17" s="4">
-        <f>G17/I17</f>
-        <v>2.6046511627906979</v>
+        <v>2.5</v>
+      </c>
+      <c r="J17" s="3">
+        <f t="shared" si="0"/>
+        <v>24</v>
       </c>
       <c r="K17">
-        <v>42.89284</v>
+        <v>42.939892</v>
       </c>
       <c r="L17">
-        <v>-123.53474</v>
+        <v>-123.00308099999999</v>
       </c>
       <c r="M17" t="s">
         <v>21</v>
       </c>
       <c r="N17" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="O17" s="1">
-        <v>43265</v>
+        <v>43297</v>
       </c>
       <c r="P17" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D18" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E18" t="s">
         <v>18</v>
@@ -1511,42 +1527,49 @@
         <v>19</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>112</v>
       </c>
       <c r="H18" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="I18">
-        <v>0.25</v>
-      </c>
-      <c r="J18" s="4">
-        <f>G18/I18</f>
-        <v>4</v>
-      </c>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="J18" s="3">
+        <f t="shared" si="0"/>
+        <v>2.6046511627906979</v>
+      </c>
+      <c r="K18">
+        <v>42.89284</v>
+      </c>
+      <c r="L18">
+        <v>-123.53474</v>
+      </c>
+      <c r="M18" t="s">
+        <v>21</v>
+      </c>
       <c r="N18" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="O18" s="1">
-        <v>43301</v>
+        <v>43265</v>
       </c>
       <c r="P18" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
         <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E19" t="s">
         <v>18</v>
@@ -1563,12 +1586,19 @@
       <c r="I19">
         <v>0.25</v>
       </c>
-      <c r="J19" s="4">
-        <f>G19/I19</f>
+      <c r="J19" s="3">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
+      <c r="K19" s="3">
+        <v>42.891894999999998</v>
+      </c>
+      <c r="L19" s="3">
+        <v>-123.535178</v>
+      </c>
+      <c r="M19" t="s">
+        <v>21</v>
+      </c>
       <c r="N19" t="s">
         <v>33</v>
       </c>
@@ -1576,27 +1606,27 @@
         <v>43301</v>
       </c>
       <c r="P19" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
         <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D20" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E20" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="F20" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -1607,15 +1637,15 @@
       <c r="I20">
         <v>0.25</v>
       </c>
-      <c r="J20">
-        <f>G20/I20</f>
+      <c r="J20" s="3">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="K20">
-        <v>42.893329999999999</v>
-      </c>
-      <c r="L20">
-        <v>-123.53346000000001</v>
+      <c r="K20" s="3">
+        <v>42.889600000000002</v>
+      </c>
+      <c r="L20" s="3">
+        <v>-123.537688</v>
       </c>
       <c r="M20" t="s">
         <v>21</v>
@@ -1624,54 +1654,112 @@
         <v>33</v>
       </c>
       <c r="O20" s="1">
-        <v>43361</v>
+        <v>43301</v>
       </c>
       <c r="P20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
         <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D21" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E21" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="F21" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="G21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H21" t="s">
         <v>20</v>
       </c>
       <c r="I21">
+        <v>0.25</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="K21">
+        <v>42.893329999999999</v>
+      </c>
+      <c r="L21">
+        <v>-123.53346000000001</v>
+      </c>
+      <c r="M21" t="s">
+        <v>21</v>
+      </c>
+      <c r="N21" t="s">
+        <v>33</v>
+      </c>
+      <c r="O21" s="1">
+        <v>43361</v>
+      </c>
+      <c r="P21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="H22" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22">
         <v>0.5</v>
       </c>
-      <c r="J21">
-        <f>G21/I21</f>
+      <c r="J22">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="N21" t="s">
+      <c r="K22" s="3">
+        <v>42.865845999999998</v>
+      </c>
+      <c r="L22" s="3">
+        <v>-123.57890399999999</v>
+      </c>
+      <c r="M22" t="s">
+        <v>21</v>
+      </c>
+      <c r="N22" t="s">
         <v>27</v>
       </c>
-      <c r="O21" s="1">
-        <v>43666</v>
-      </c>
-      <c r="P21" s="2" t="s">
-        <v>76</v>
+      <c r="O22" s="1">
+        <v>43301</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1694,7 +1782,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1707,7 +1795,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1735,7 +1823,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -1743,7 +1831,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1751,7 +1839,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>